<commit_message>
update scripts & dataframes
</commit_message>
<xml_diff>
--- a/derivatives/imaging_plots/istart_covariates_socialdoors_2.xlsx
+++ b/derivatives/imaging_plots/istart_covariates_socialdoors_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/Documents_Air/GitHub/istart-socdoors/derivatives/imaging_plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6447F72-C657-DE4F-8296-CF04980F9B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB08A119-8001-8A4A-B84F-977E703E65A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1220" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model-2 social" sheetId="8" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>